<commit_message>
fix bug where output tower tables were using slightly different material properties
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/WISDEM/outputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451AC20E-AD08-B242-B318-F35C78A2F077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54633118-741D-7342-8349-282043745806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20067,7 +20067,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20142,16 +20142,16 @@
         <v>167787.53027957</v>
       </c>
       <c r="H2">
-        <v>4274841535785.2231</v>
+        <v>4488583612574.4844</v>
       </c>
       <c r="I2">
-        <v>4274841535785.2231</v>
+        <v>4488583612574.4844</v>
       </c>
       <c r="J2">
         <v>3389949337877.6821</v>
       </c>
       <c r="K2">
-        <v>345793453239.61108</v>
+        <v>363083125901.59167</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -20177,16 +20177,16 @@
         <v>167787.53027957</v>
       </c>
       <c r="H3">
-        <v>4274841535785.2231</v>
+        <v>4488583612574.4844</v>
       </c>
       <c r="I3">
-        <v>4274841535785.2231</v>
+        <v>4488583612574.4844</v>
       </c>
       <c r="J3">
         <v>3389949337877.6821</v>
       </c>
       <c r="K3">
-        <v>345793453239.61108</v>
+        <v>363083125901.59167</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -20209,16 +20209,16 @@
         <v>167787.53027957</v>
       </c>
       <c r="H4">
-        <v>4274841535785.2231</v>
+        <v>4488583612574.4844</v>
       </c>
       <c r="I4">
-        <v>4274841535785.2231</v>
+        <v>4488583612574.4844</v>
       </c>
       <c r="J4">
         <v>3389949337877.6821</v>
       </c>
       <c r="K4">
-        <v>345793453239.61108</v>
+        <v>363083125901.59167</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -20241,16 +20241,16 @@
         <v>167787.53027957</v>
       </c>
       <c r="H5">
-        <v>4274841535785.2231</v>
+        <v>4488583612574.4844</v>
       </c>
       <c r="I5">
-        <v>4274841535785.2231</v>
+        <v>4488583612574.4844</v>
       </c>
       <c r="J5">
         <v>3389949337877.6821</v>
       </c>
       <c r="K5">
-        <v>345793453239.61108</v>
+        <v>363083125901.59167</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -20273,16 +20273,16 @@
         <v>162143.3749428468</v>
       </c>
       <c r="H6">
-        <v>4131041399817.752</v>
+        <v>4337593469808.6401</v>
       </c>
       <c r="I6">
-        <v>4131041399817.752</v>
+        <v>4337593469808.6401</v>
       </c>
       <c r="J6">
         <v>3275915830055.478</v>
       </c>
       <c r="K6">
-        <v>334034993868.85773</v>
+        <v>350736743562.3006</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -20305,16 +20305,16 @@
         <v>162143.3749428468</v>
       </c>
       <c r="H7">
-        <v>4131041399817.752</v>
+        <v>4337593469808.6401</v>
       </c>
       <c r="I7">
-        <v>4131041399817.752</v>
+        <v>4337593469808.6401</v>
       </c>
       <c r="J7">
         <v>3275915830055.478</v>
       </c>
       <c r="K7">
-        <v>334034993868.85773</v>
+        <v>350736743562.3006</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -20337,16 +20337,16 @@
         <v>156349.29857748951</v>
       </c>
       <c r="H8">
-        <v>3983421619808.6509</v>
+        <v>4182592700799.083</v>
       </c>
       <c r="I8">
-        <v>3983421619808.6509</v>
+        <v>4182592700799.083</v>
       </c>
       <c r="J8">
         <v>3158853344508.2598</v>
       </c>
       <c r="K8">
-        <v>321973551662.24689</v>
+        <v>338072229245.35931</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -20369,16 +20369,16 @@
         <v>156349.29857748951</v>
       </c>
       <c r="H9">
-        <v>3983421619808.6509</v>
+        <v>4182592700799.083</v>
       </c>
       <c r="I9">
-        <v>3983421619808.6509</v>
+        <v>4182592700799.083</v>
       </c>
       <c r="J9">
         <v>3158853344508.2598</v>
       </c>
       <c r="K9">
-        <v>321973551662.24689</v>
+        <v>338072229245.35931</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -20401,16 +20401,16 @@
         <v>150422.74186629331</v>
       </c>
       <c r="H10">
-        <v>3832426544364.1611</v>
+        <v>4024047871582.3691</v>
       </c>
       <c r="I10">
-        <v>3832426544364.1611</v>
+        <v>4024047871582.3691</v>
       </c>
       <c r="J10">
         <v>3039114249680.7788</v>
       </c>
       <c r="K10">
-        <v>309646101275.31641</v>
+        <v>325128406339.08221</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -20433,16 +20433,16 @@
         <v>150422.74186629331</v>
       </c>
       <c r="H11">
-        <v>3832426544364.1611</v>
+        <v>4024047871582.3691</v>
       </c>
       <c r="I11">
-        <v>3832426544364.1611</v>
+        <v>4024047871582.3691</v>
       </c>
       <c r="J11">
         <v>3039114249680.7788</v>
       </c>
       <c r="K11">
-        <v>309646101275.31641</v>
+        <v>325128406339.08221</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -20465,16 +20465,16 @@
         <v>144405.1855129351</v>
       </c>
       <c r="H12">
-        <v>3679113006698.9839</v>
+        <v>3863068657033.9341</v>
       </c>
       <c r="I12">
-        <v>3679113006698.9839</v>
+        <v>3863068657033.9341</v>
       </c>
       <c r="J12">
         <v>2917536614312.2939</v>
       </c>
       <c r="K12">
-        <v>297139457640.30811</v>
+        <v>311996430522.32349</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -20497,16 +20497,16 @@
         <v>144405.1855129351</v>
       </c>
       <c r="H13">
-        <v>3679113006698.9839</v>
+        <v>3863068657033.9341</v>
       </c>
       <c r="I13">
-        <v>3679113006698.9839</v>
+        <v>3863068657033.9341</v>
       </c>
       <c r="J13">
         <v>2917536614312.2939</v>
       </c>
       <c r="K13">
-        <v>297139457640.30811</v>
+        <v>311996430522.32349</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -20529,16 +20529,16 @@
         <v>138410.2906162251</v>
       </c>
       <c r="H14">
-        <v>3526376830986.626</v>
+        <v>3702695672535.958</v>
       </c>
       <c r="I14">
-        <v>3526376830986.626</v>
+        <v>3702695672535.958</v>
       </c>
       <c r="J14">
         <v>2796416826972.395</v>
       </c>
       <c r="K14">
-        <v>284689996998.32593</v>
+        <v>298924496848.24219</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -20564,16 +20564,16 @@
         <v>138410.2906162251</v>
       </c>
       <c r="H15">
-        <v>3526376830986.626</v>
+        <v>3702695672535.958</v>
       </c>
       <c r="I15">
-        <v>3526376830986.626</v>
+        <v>3702695672535.958</v>
       </c>
       <c r="J15">
         <v>2796416826972.395</v>
       </c>
       <c r="K15">
-        <v>284689996998.32593</v>
+        <v>298924496848.24219</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -20596,16 +20596,16 @@
         <v>132438.16023370199</v>
       </c>
       <c r="H16">
-        <v>3374220642896.8662</v>
+        <v>3542931675041.709</v>
       </c>
       <c r="I16">
-        <v>3374220642896.8662</v>
+        <v>3542931675041.709</v>
       </c>
       <c r="J16">
         <v>2675756969817.2139</v>
       </c>
       <c r="K16">
-        <v>272297794747.58209</v>
+        <v>285912684484.96118</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -20628,16 +20628,16 @@
         <v>132438.16023370199</v>
       </c>
       <c r="H17">
-        <v>3374220642896.8662</v>
+        <v>3542931675041.709</v>
       </c>
       <c r="I17">
-        <v>3374220642896.8662</v>
+        <v>3542931675041.709</v>
       </c>
       <c r="J17">
         <v>2675756969817.2139</v>
       </c>
       <c r="K17">
-        <v>272297794747.58209</v>
+        <v>285912684484.96118</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -20660,16 +20660,16 @@
         <v>128577.9604820947</v>
       </c>
       <c r="H18">
-        <v>3275871604639.355</v>
+        <v>3439665184871.3232</v>
       </c>
       <c r="I18">
-        <v>3275871604639.355</v>
+        <v>3439665184871.3232</v>
       </c>
       <c r="J18">
         <v>2597766182479.0088</v>
       </c>
       <c r="K18">
-        <v>264293150601.75339</v>
+        <v>277507808131.84113</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -20692,16 +20692,16 @@
         <v>128577.9604820947</v>
       </c>
       <c r="H19">
-        <v>3275871604639.355</v>
+        <v>3439665184871.3232</v>
       </c>
       <c r="I19">
-        <v>3275871604639.355</v>
+        <v>3439665184871.3232</v>
       </c>
       <c r="J19">
         <v>2597766182479.0088</v>
       </c>
       <c r="K19">
-        <v>264293150601.75339</v>
+        <v>277507808131.84113</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -20724,16 +20724,16 @@
         <v>125018.51146756471</v>
       </c>
       <c r="H20">
-        <v>3185185005543.0488</v>
+        <v>3344444255820.2012</v>
       </c>
       <c r="I20">
-        <v>3185185005543.0488</v>
+        <v>3344444255820.2012</v>
       </c>
       <c r="J20">
         <v>2525851709395.6382</v>
       </c>
       <c r="K20">
-        <v>256915828495.4436</v>
+        <v>269761619920.21579</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -20759,16 +20759,16 @@
         <v>125018.51146756471</v>
       </c>
       <c r="H21">
-        <v>3185185005543.0488</v>
+        <v>3344444255820.2012</v>
       </c>
       <c r="I21">
-        <v>3185185005543.0488</v>
+        <v>3344444255820.2012</v>
       </c>
       <c r="J21">
         <v>2525851709395.6382</v>
       </c>
       <c r="K21">
-        <v>256915828495.4436</v>
+        <v>269761619920.21579</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -20791,16 +20791,16 @@
         <v>120318.7822579303</v>
       </c>
       <c r="H22">
-        <v>3065446681730.708</v>
+        <v>3218719015817.2441</v>
       </c>
       <c r="I22">
-        <v>3065446681730.708</v>
+        <v>3218719015817.2441</v>
       </c>
       <c r="J22">
         <v>2430899218612.4521</v>
       </c>
       <c r="K22">
-        <v>247180551443.41281</v>
+        <v>259539579015.5834</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -20823,16 +20823,16 @@
         <v>120318.7822579303</v>
       </c>
       <c r="H23">
-        <v>3065446681730.708</v>
+        <v>3218719015817.2441</v>
       </c>
       <c r="I23">
-        <v>3065446681730.708</v>
+        <v>3218719015817.2441</v>
       </c>
       <c r="J23">
         <v>2430899218612.4521</v>
       </c>
       <c r="K23">
-        <v>247180551443.41281</v>
+        <v>259539579015.5834</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -20855,16 +20855,16 @@
         <v>111159.32510666719</v>
       </c>
       <c r="H24">
-        <v>2832084716093.4321</v>
+        <v>2973688951898.104</v>
       </c>
       <c r="I24">
-        <v>2832084716093.4321</v>
+        <v>2973688951898.104</v>
       </c>
       <c r="J24">
         <v>2245843179862.0918</v>
       </c>
       <c r="K24">
-        <v>228224743138.6868</v>
+        <v>239635980295.62119</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -20887,16 +20887,16 @@
         <v>108700.9302411078</v>
       </c>
       <c r="H25">
-        <v>2769450452002.7461</v>
+        <v>2907922974602.8828</v>
       </c>
       <c r="I25">
-        <v>2769450452002.7461</v>
+        <v>2907922974602.8828</v>
       </c>
       <c r="J25">
         <v>2196174208438.178</v>
       </c>
       <c r="K25">
-        <v>226529700592.35431</v>
+        <v>237856185621.97198</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -20919,16 +20919,16 @@
         <v>100800.53234512761</v>
       </c>
       <c r="H26">
-        <v>2568166429175.2251</v>
+        <v>2696574750633.9858</v>
       </c>
       <c r="I26">
-        <v>2568166429175.2251</v>
+        <v>2696574750633.9858</v>
       </c>
       <c r="J26">
         <v>2036555978335.9529</v>
       </c>
       <c r="K26">
-        <v>209952218050.84689</v>
+        <v>220449828953.38919</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -20951,16 +20951,16 @@
         <v>86744.69725724234</v>
       </c>
       <c r="H27">
-        <v>2210055981076.2378</v>
+        <v>2320558780130.0498</v>
       </c>
       <c r="I27">
-        <v>2210055981076.2378</v>
+        <v>2320558780130.0498</v>
       </c>
       <c r="J27">
         <v>1752574392993.457</v>
       </c>
       <c r="K27">
-        <v>199701039744.32401</v>
+        <v>209686091731.54019</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -20983,16 +20983,16 @@
         <v>82711.009666520113</v>
       </c>
       <c r="H28">
-        <v>2107286870484.5891</v>
+        <v>2212651214008.8179</v>
       </c>
       <c r="I28">
-        <v>2107286870484.5891</v>
+        <v>2212651214008.8179</v>
       </c>
       <c r="J28">
         <v>1671078488294.2791</v>
       </c>
       <c r="K28">
-        <v>190350814904.366</v>
+        <v>199868355649.58429</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -21015,16 +21015,16 @@
         <v>67647.375429982465</v>
       </c>
       <c r="H29">
-        <v>1723500010954.967</v>
+        <v>1809675011502.7161</v>
       </c>
       <c r="I29">
-        <v>1723500010954.967</v>
+        <v>1809675011502.7161</v>
       </c>
       <c r="J29">
         <v>1366735508687.2891</v>
       </c>
       <c r="K29">
-        <v>178012448518.43231</v>
+        <v>186913070944.35391</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -21047,16 +21047,16 @@
         <v>64561.509227087583</v>
       </c>
       <c r="H30">
-        <v>1644879215976.7529</v>
+        <v>1727123176775.5911</v>
       </c>
       <c r="I30">
-        <v>1644879215976.7529</v>
+        <v>1727123176775.5911</v>
       </c>
       <c r="J30">
         <v>1304389218269.5649</v>
       </c>
       <c r="K30">
-        <v>169834990660.59619</v>
+        <v>178326740193.62589</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -21079,16 +21079,16 @@
         <v>50687.657897153673</v>
       </c>
       <c r="H31">
-        <v>1291405296742.769</v>
+        <v>1355975561579.907</v>
       </c>
       <c r="I31">
-        <v>1291405296742.769</v>
+        <v>1355975561579.907</v>
       </c>
       <c r="J31">
         <v>1024084400317.016</v>
       </c>
       <c r="K31">
-        <v>156676206149.63971</v>
+        <v>164510016457.1217</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -21111,16 +21111,16 @@
         <v>48063.543306744883</v>
       </c>
       <c r="H32">
-        <v>1224548874057.1941</v>
+        <v>1285776317760.054</v>
       </c>
       <c r="I32">
-        <v>1224548874057.1941</v>
+        <v>1285776317760.054</v>
       </c>
       <c r="J32">
         <v>971067257127.3551</v>
       </c>
       <c r="K32">
-        <v>148506466847.54681</v>
+        <v>155931790189.9241</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -21143,16 +21143,16 @@
         <v>35779.710273115757</v>
       </c>
       <c r="H33">
-        <v>911584975111.22949</v>
+        <v>957164223866.79102</v>
       </c>
       <c r="I33">
-        <v>911584975111.22949</v>
+        <v>957164223866.79102</v>
       </c>
       <c r="J33">
         <v>722886885263.20496</v>
       </c>
       <c r="K33">
-        <v>134591812002.54359</v>
+        <v>141321402602.67068</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -21175,16 +21175,16 @@
         <v>33484.09822793756</v>
       </c>
       <c r="H34">
-        <v>853098044023.88684</v>
+        <v>895752946225.08118</v>
       </c>
       <c r="I34">
-        <v>853098044023.88684</v>
+        <v>895752946225.08118</v>
       </c>
       <c r="J34">
         <v>676506748910.94226</v>
       </c>
       <c r="K34">
-        <v>125892114148.985</v>
+        <v>132186719856.4342</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -21207,16 +21207,16 @@
         <v>27341.12841421437</v>
       </c>
       <c r="H35">
-        <v>696589258960.87573</v>
+        <v>731418721908.91956</v>
       </c>
       <c r="I35">
-        <v>696589258960.87573</v>
+        <v>731418721908.91956</v>
       </c>
       <c r="J35">
         <v>552395282355.97449</v>
       </c>
       <c r="K35">
-        <v>117667768272.1226</v>
+        <v>123551156685.7287</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -21239,16 +21239,16 @@
         <v>24155.666545742861</v>
       </c>
       <c r="H36">
-        <v>615430994795.99658</v>
+        <v>646202544535.79639</v>
       </c>
       <c r="I36">
-        <v>615430994795.99658</v>
+        <v>646202544535.79639</v>
       </c>
       <c r="J36">
         <v>488036778873.22522</v>
       </c>
       <c r="K36">
-        <v>103862152005.8945</v>
+        <v>109055259606.18919</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -21271,16 +21271,16 @@
         <v>22500.414643593769</v>
       </c>
       <c r="H37">
-        <v>573258971811.30627</v>
+        <v>601921920401.87158</v>
       </c>
       <c r="I37">
-        <v>573258971811.30627</v>
+        <v>601921920401.87158</v>
       </c>
       <c r="J37">
         <v>454594364646.36578</v>
       </c>
       <c r="K37">
-        <v>101433418769.6498</v>
+        <v>106505089708.13229</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -21303,16 +21303,16 @@
         <v>19545.084466970689</v>
       </c>
       <c r="H38">
-        <v>497963935464.22137</v>
+        <v>522862132237.4325</v>
       </c>
       <c r="I38">
-        <v>497963935464.22137</v>
+        <v>522862132237.4325</v>
       </c>
       <c r="J38">
         <v>394885400823.12762</v>
       </c>
       <c r="K38">
-        <v>88027505148.305237</v>
+        <v>92428880405.72049</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -21335,16 +21335,16 @@
         <v>18050.83094737371</v>
       </c>
       <c r="H39">
-        <v>459893782098.69342</v>
+        <v>482888471203.62811</v>
       </c>
       <c r="I39">
-        <v>459893782098.69342</v>
+        <v>482888471203.62811</v>
       </c>
       <c r="J39">
         <v>364695769204.26392</v>
       </c>
       <c r="K39">
-        <v>85724481485.455917</v>
+        <v>90010705559.728714</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -21367,16 +21367,16 @@
         <v>20770.01618251999</v>
       </c>
       <c r="H40">
-        <v>529172386815.79602</v>
+        <v>555631006156.58582</v>
       </c>
       <c r="I40">
-        <v>529172386815.79602</v>
+        <v>555631006156.58582</v>
       </c>
       <c r="J40">
         <v>419633702744.92621</v>
       </c>
       <c r="K40">
-        <v>98733315436.687683</v>
+        <v>103669981208.52209</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -21402,16 +21402,16 @@
         <v>20092.38437489187</v>
       </c>
       <c r="H41">
-        <v>511907882162.8501</v>
+        <v>537503276270.99261</v>
       </c>
       <c r="I41">
-        <v>511907882162.8501</v>
+        <v>537503276270.99261</v>
       </c>
       <c r="J41">
         <v>405942950555.14008</v>
       </c>
       <c r="K41">
-        <v>97647671493.475189</v>
+        <v>102530055068.1489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding readmes to individual folders and correcting error in nacelle mass and cm
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/systems/referenceTurbines/15mw/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B3AD04-D7E9-3241-841C-8325648557EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21931387-AC97-0E40-B9A9-CE0D9A301092}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20120" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1235,9 +1235,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1536,9 +1542,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D329"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -4889,9 +4903,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -14349,9 +14382,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F158"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -16922,9 +16965,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -17979,9 +18031,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AQ39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -21297,9 +21388,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -23856,9 +23961,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="93" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="97.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -24515,9 +24634,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -26032,11 +26164,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
@@ -26715,9 +26857,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G214"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -31455,9 +31608,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -32364,9 +32525,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D408"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -36823,9 +36992,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D329"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -40176,9 +40353,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D329"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -43529,9 +43714,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D386"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -47338,9 +47531,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D329"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -50691,9 +50892,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D386"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
update nacelle properties to make the consistency with openfast more transparent
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>10.66821594497437</v>
+        <v>10.65319618433997</v>
       </c>
     </row>
     <row r="11">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9575621690059503</v>
+        <v>0.9575621467294017</v>
       </c>
     </row>
     <row r="25">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>69867.33094009876</v>
+        <v>69549.16141249203</v>
       </c>
     </row>
     <row r="27">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>21761.60830103885</v>
+        <v>21788.17237526133</v>
       </c>
     </row>
     <row r="28">
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>673650.212437295</v>
+        <v>673650.1955449819</v>
       </c>
     </row>
     <row r="30">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>952032.5574975831</v>
+        <v>951046.3196540715</v>
       </c>
     </row>
     <row r="31">
@@ -25423,16 +25423,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>3.843913007233334</v>
+        <v>3.869872082015147</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0418599144610877</v>
+        <v>0.0388246469088558</v>
       </c>
       <c r="D2" t="n">
-        <v>0.05558440248889981</v>
+        <v>0.05155404577270924</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05809086607852369</v>
+        <v>0.05387876864235928</v>
       </c>
       <c r="F2" t="n">
         <v>4.999999999999999</v>
@@ -25441,22 +25441,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H2" t="n">
-        <v>0.204216801952453</v>
+        <v>0.2051946760772687</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8135183070146771</v>
+        <v>0.8174149591859494</v>
       </c>
       <c r="J2" t="n">
-        <v>0.08355157175087501</v>
+        <v>0.07749323681438851</v>
       </c>
       <c r="K2" t="n">
-        <v>0.002764506728362953</v>
+        <v>0.002564057605738348</v>
       </c>
       <c r="L2" t="n">
-        <v>5.983183452008846</v>
+        <v>6.039279674114795</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1979681598262107</v>
+        <v>0.1998246765544819</v>
       </c>
     </row>
     <row r="3">
@@ -25464,16 +25464,16 @@
         <v>3.549532370424899</v>
       </c>
       <c r="B3" t="n">
-        <v>3.83768586301179</v>
+        <v>3.860526788392669</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2926826196884224</v>
+        <v>0.2913918300921703</v>
       </c>
       <c r="D3" t="n">
-        <v>0.234639907799418</v>
+        <v>0.2336054388499749</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2452205088176514</v>
+        <v>0.2441393920641114</v>
       </c>
       <c r="F3" t="n">
         <v>4.999999999999999</v>
@@ -25482,22 +25482,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2766415680235341</v>
+        <v>0.278224093891547</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7872152966323006</v>
+        <v>0.7917197095446022</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5841887928811563</v>
+        <v>0.5816124007031206</v>
       </c>
       <c r="K3" t="n">
-        <v>0.01380754526029661</v>
+        <v>0.01374668121772323</v>
       </c>
       <c r="L3" t="n">
-        <v>7.840006617773356</v>
+        <v>7.918952253517621</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1853018194375949</v>
+        <v>0.187168141662516</v>
       </c>
     </row>
     <row r="4">
@@ -25505,16 +25505,16 @@
         <v>4.067900770958515</v>
       </c>
       <c r="B4" t="n">
-        <v>3.644704741536342</v>
+        <v>3.662763557193586</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6095877216459016</v>
+        <v>0.6102732106870125</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3246710221631849</v>
+        <v>0.3250365926235918</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3393113899501824</v>
+        <v>0.3396934442638405</v>
       </c>
       <c r="F4" t="n">
         <v>4.999999999999999</v>
@@ -25523,22 +25523,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3604174985164955</v>
+        <v>0.3627977373137081</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7808786269740569</v>
+        <v>0.7860367854833162</v>
       </c>
       <c r="J4" t="n">
-        <v>1.216725187312447</v>
+        <v>1.218093407218049</v>
       </c>
       <c r="K4" t="n">
-        <v>0.02189562436813417</v>
+        <v>0.02192029415295585</v>
       </c>
       <c r="L4" t="n">
-        <v>9.997951659987732</v>
+        <v>10.1056196243703</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1799185192191142</v>
+        <v>0.1818564598178033</v>
       </c>
     </row>
     <row r="5">
@@ -25546,16 +25546,16 @@
         <v>4.553906848103765</v>
       </c>
       <c r="B5" t="n">
-        <v>3.29302686361453</v>
+        <v>3.306551411726073</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9845331773210557</v>
+        <v>0.9873300221875337</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3737629912625884</v>
+        <v>0.3748253171227007</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3906170597926165</v>
+        <v>0.3917272881276658</v>
       </c>
       <c r="F5" t="n">
         <v>4.999999999999999</v>
@@ -25564,22 +25564,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4528032293250858</v>
+        <v>0.4560867938652214</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7828158298386281</v>
+        <v>0.7884936753096888</v>
       </c>
       <c r="J5" t="n">
-        <v>1.965108994250909</v>
+        <v>1.970691437399317</v>
       </c>
       <c r="K5" t="n">
-        <v>0.02821784831328822</v>
+        <v>0.0282980709014952</v>
       </c>
       <c r="L5" t="n">
-        <v>12.38404024014955</v>
+        <v>12.52379735874302</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1778277795402421</v>
+        <v>0.1798350055660475</v>
       </c>
     </row>
     <row r="6">
@@ -25587,16 +25587,16 @@
         <v>5.006427062922798</v>
       </c>
       <c r="B6" t="n">
-        <v>2.861421634573576</v>
+        <v>2.872738038213265</v>
       </c>
       <c r="C6" t="n">
-        <v>1.406815635465982</v>
+        <v>1.411956072923998</v>
       </c>
       <c r="D6" t="n">
-        <v>0.401949854006695</v>
+        <v>0.4034191477510797</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4200749507750484</v>
+        <v>0.4216104982993255</v>
       </c>
       <c r="F6" t="n">
         <v>4.999999999999999</v>
@@ -25605,22 +25605,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H6" t="n">
-        <v>0.548410802795122</v>
+        <v>0.5525363345777579</v>
       </c>
       <c r="I6" t="n">
-        <v>0.7844559895857482</v>
+        <v>0.7903583714314903</v>
       </c>
       <c r="J6" t="n">
-        <v>2.807976533639447</v>
+        <v>2.818236739859587</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0333613198310383</v>
+        <v>0.03348329364542108</v>
       </c>
       <c r="L6" t="n">
-        <v>14.85580702689507</v>
+        <v>15.02645488382177</v>
       </c>
       <c r="M6" t="n">
-        <v>0.1765005240019112</v>
+        <v>0.1785283664103193</v>
       </c>
     </row>
     <row r="7">
@@ -25628,16 +25628,16 @@
         <v>5.424415288411413</v>
       </c>
       <c r="B7" t="n">
-        <v>2.378036902446298</v>
+        <v>2.387009689822399</v>
       </c>
       <c r="C7" t="n">
-        <v>1.864187363751022</v>
+        <v>1.871782902213637</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4187445184373225</v>
+        <v>0.4204512850119446</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4376269358389906</v>
+        <v>0.4394106644978981</v>
       </c>
       <c r="F7" t="n">
         <v>4.999999999999999</v>
@@ -25646,22 +25646,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6446009956476877</v>
+        <v>0.6496064755978329</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7854227533994075</v>
+        <v>0.7915229016148269</v>
       </c>
       <c r="J7" t="n">
-        <v>3.720881570943152</v>
+        <v>3.736042108686354</v>
       </c>
       <c r="K7" t="n">
-        <v>0.03765698291650161</v>
+        <v>0.03781049700525153</v>
       </c>
       <c r="L7" t="n">
-        <v>17.34609884992052</v>
+        <v>17.54924442922418</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1755502656038135</v>
+        <v>0.1776065779325277</v>
       </c>
     </row>
     <row r="8">
@@ -25669,16 +25669,16 @@
         <v>5.806905227914102</v>
       </c>
       <c r="B8" t="n">
-        <v>1.878150799903513</v>
+        <v>1.885886577973215</v>
       </c>
       <c r="C8" t="n">
-        <v>2.342781816237434</v>
+        <v>2.352790381450226</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4289592123855399</v>
+        <v>0.4307923909855927</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4483022402698965</v>
+        <v>0.4502180812177562</v>
       </c>
       <c r="F8" t="n">
         <v>4.999999999999999</v>
@@ -25687,22 +25687,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H8" t="n">
-        <v>0.7382803329148493</v>
+        <v>0.7440869513790228</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7849648180916245</v>
+        <v>0.7911397660766929</v>
       </c>
       <c r="J8" t="n">
-        <v>4.676146751278405</v>
+        <v>4.696123641056215</v>
       </c>
       <c r="K8" t="n">
-        <v>0.04129563916498331</v>
+        <v>0.04147214827128595</v>
       </c>
       <c r="L8" t="n">
-        <v>19.77477164826465</v>
+        <v>20.00871418493256</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1746334916314221</v>
+        <v>0.1766998539264764</v>
       </c>
     </row>
     <row r="9">
@@ -25710,16 +25710,16 @@
         <v>6.153012648988982</v>
       </c>
       <c r="B9" t="n">
-        <v>1.384817322059855</v>
+        <v>1.390984514024913</v>
       </c>
       <c r="C9" t="n">
-        <v>2.82774197989467</v>
+        <v>2.840042147155181</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4352058503104329</v>
+        <v>0.4370995543956271</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4548305574036186</v>
+        <v>0.4568096530927745</v>
       </c>
       <c r="F9" t="n">
         <v>4.999999999999999</v>
@@ -25728,22 +25728,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8271201360887537</v>
+        <v>0.8336974334645489</v>
       </c>
       <c r="I9" t="n">
-        <v>0.783269737010008</v>
+        <v>0.7894994848888429</v>
       </c>
       <c r="J9" t="n">
-        <v>5.644117766789908</v>
+        <v>5.668668647238624</v>
       </c>
       <c r="K9" t="n">
-        <v>0.04439417479871843</v>
+        <v>0.04458737883904663</v>
       </c>
       <c r="L9" t="n">
-        <v>22.08202892055931</v>
+        <v>22.34654157238428</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1736876323839038</v>
+        <v>0.1757685581632586</v>
       </c>
     </row>
     <row r="10">
@@ -25751,16 +25751,16 @@
         <v>6.461937427558303</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9114566713334133</v>
+        <v>0.9166701805514654</v>
       </c>
       <c r="C10" t="n">
-        <v>3.303695500162815</v>
+        <v>3.318119851622634</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4389652445458862</v>
+        <v>0.4408824648953117</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4587594737414654</v>
+        <v>0.4607631461029226</v>
       </c>
       <c r="F10" t="n">
         <v>4.999999999999999</v>
@@ -25769,22 +25769,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9094424331952713</v>
+        <v>0.91669860341597</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7808508481215498</v>
+        <v>0.7870821717668562</v>
       </c>
       <c r="J10" t="n">
-        <v>6.594111697994231</v>
+        <v>6.622902406400643</v>
       </c>
       <c r="K10" t="n">
-        <v>0.04702581590095951</v>
+        <v>0.04723123971477182</v>
       </c>
       <c r="L10" t="n">
-        <v>24.22621362876093</v>
+        <v>24.5188946089825</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1727689056935391</v>
+        <v>0.1748565383809498</v>
       </c>
     </row>
     <row r="11">
@@ -25792,16 +25792,16 @@
         <v>6.732965397618989</v>
       </c>
       <c r="B11" t="n">
-        <v>0.4689317546207939</v>
+        <v>0.4735234175757265</v>
       </c>
       <c r="C11" t="n">
-        <v>3.755595748533946</v>
+        <v>3.77190142553299</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4411416470202074</v>
+        <v>0.4430575983918076</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4610340165809608</v>
+        <v>0.463036362737377</v>
       </c>
       <c r="F11" t="n">
         <v>4.999999999999999</v>
@@ -25810,22 +25810,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9838881482506596</v>
+        <v>0.991768083977042</v>
       </c>
       <c r="I11" t="n">
-        <v>0.7781285197561888</v>
+        <v>0.7843616751360892</v>
       </c>
       <c r="J11" t="n">
-        <v>7.496095768246382</v>
+        <v>7.528641563580721</v>
       </c>
       <c r="K11" t="n">
-        <v>0.04924111720857992</v>
+        <v>0.04945501548274017</v>
       </c>
       <c r="L11" t="n">
-        <v>26.17312837945665</v>
+        <v>26.49169175368979</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1719287109040673</v>
+        <v>0.1740217029564076</v>
       </c>
     </row>
     <row r="12">
@@ -25833,16 +25833,16 @@
         <v>6.965470002237022</v>
       </c>
       <c r="B12" t="n">
-        <v>0.07017895977653038</v>
+        <v>0.07652063393802891</v>
       </c>
       <c r="C12" t="n">
-        <v>4.169206503707341</v>
+        <v>4.187008206224884</v>
       </c>
       <c r="D12" t="n">
-        <v>0.442303623289134</v>
+        <v>0.4441928214310457</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4622483897648431</v>
+        <v>0.4642227763072886</v>
       </c>
       <c r="F12" t="n">
         <v>4.999999999999999</v>
@@ -25851,22 +25851,22 @@
         <v>63.41769634044945</v>
       </c>
       <c r="H12" t="n">
-        <v>1.049164808077995</v>
+        <v>1.057454491807478</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7752847321908845</v>
+        <v>0.7814115678303072</v>
       </c>
       <c r="J12" t="n">
-        <v>8.321654757859891</v>
+        <v>8.357186588985135</v>
       </c>
       <c r="K12" t="n">
-        <v>0.05107570598611944</v>
+        <v>0.05129390137805238</v>
       </c>
       <c r="L12" t="n">
-        <v>27.88806423850027</v>
+        <v>28.22575729419021</v>
       </c>
       <c r="M12" t="n">
-        <v>0.1711681884209734</v>
+        <v>0.1732412212594683</v>
       </c>
     </row>
     <row r="13">
@@ -25877,37 +25877,37 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>4.535731192111332</v>
+        <v>4.554986629627561</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4432250408100386</v>
+        <v>0.4451073029531735</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4624857984125064</v>
+        <v>0.4644498266902297</v>
       </c>
       <c r="F13" t="n">
-        <v>5.086085279081918</v>
+        <v>5.086088977638215</v>
       </c>
       <c r="G13" t="n">
-        <v>64.50956235808945</v>
+        <v>64.50960926887348</v>
       </c>
       <c r="H13" t="n">
-        <v>1.10306475219421</v>
+        <v>1.112185726327055</v>
       </c>
       <c r="I13" t="n">
-        <v>0.7716584514413148</v>
+        <v>0.7780402416718009</v>
       </c>
       <c r="J13" t="n">
-        <v>8.886058445015371</v>
+        <v>8.923775176192317</v>
       </c>
       <c r="K13" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.05185144301213621</v>
       </c>
       <c r="L13" t="n">
-        <v>29.30931759530399</v>
+        <v>29.67605662499316</v>
       </c>
       <c r="M13" t="n">
-        <v>0.1703009161402403</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="14">
@@ -25918,37 +25918,37 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>4.843106047222089</v>
+        <v>4.863666353909917</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4439994739629508</v>
+        <v>0.4458850228716393</v>
       </c>
       <c r="E14" t="n">
-        <v>0.4624857984125063</v>
+        <v>0.4644498266902298</v>
       </c>
       <c r="F14" t="n">
-        <v>5.195449632666688</v>
+        <v>5.195453410751776</v>
       </c>
       <c r="G14" t="n">
-        <v>65.89668943131115</v>
+        <v>65.89673735080171</v>
       </c>
       <c r="H14" t="n">
-        <v>1.151012418756607</v>
+        <v>1.160529860481745</v>
       </c>
       <c r="I14" t="n">
-        <v>0.7716584514413148</v>
+        <v>0.7780402416718007</v>
       </c>
       <c r="J14" t="n">
-        <v>9.272314797172433</v>
+        <v>9.311670987181422</v>
       </c>
       <c r="K14" t="n">
-        <v>0.05163217769028857</v>
+        <v>0.05185144301213623</v>
       </c>
       <c r="L14" t="n">
-        <v>30.583325657329</v>
+        <v>30.96600598210167</v>
       </c>
       <c r="M14" t="n">
-        <v>0.1703009161402403</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="15">
@@ -25959,37 +25959,37 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>5.078705235977451</v>
+        <v>5.100265686034393</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4444725398331866</v>
+        <v>0.4463600942734645</v>
       </c>
       <c r="E15" t="n">
-        <v>0.4624857984125061</v>
+        <v>0.4644498266902297</v>
       </c>
       <c r="F15" t="n">
-        <v>5.276492462585394</v>
+        <v>5.276496299604113</v>
       </c>
       <c r="G15" t="n">
-        <v>66.92459934698219</v>
+        <v>66.92464801395978</v>
       </c>
       <c r="H15" t="n">
-        <v>1.187201333666708</v>
+        <v>1.197018012726857</v>
       </c>
       <c r="I15" t="n">
-        <v>0.7716584514413146</v>
+        <v>0.7780402416718006</v>
       </c>
       <c r="J15" t="n">
-        <v>9.563845110613387</v>
+        <v>9.604438696316992</v>
       </c>
       <c r="K15" t="n">
-        <v>0.05163217769028855</v>
+        <v>0.05185144301213621</v>
       </c>
       <c r="L15" t="n">
-        <v>31.54489423108652</v>
+        <v>31.93960638582497</v>
       </c>
       <c r="M15" t="n">
-        <v>0.1703009161402403</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="16">
@@ -26000,37 +26000,37 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>5.235225766907385</v>
+        <v>5.257450655130001</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4447538228627595</v>
+        <v>0.4466425690340009</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4624857984125061</v>
+        <v>0.4644498266902296</v>
       </c>
       <c r="F16" t="n">
-        <v>5.329026415676567</v>
+        <v>5.329030290897512</v>
       </c>
       <c r="G16" t="n">
-        <v>67.59091580392206</v>
+        <v>67.59096495543909</v>
       </c>
       <c r="H16" t="n">
-        <v>1.210959107023136</v>
+        <v>1.220972233332467</v>
       </c>
       <c r="I16" t="n">
-        <v>0.7716584514413147</v>
+        <v>0.7780402416718007</v>
       </c>
       <c r="J16" t="n">
-        <v>9.755232753223401</v>
+        <v>9.796638680676903</v>
       </c>
       <c r="K16" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.05185144301213621</v>
       </c>
       <c r="L16" t="n">
-        <v>32.17615737613369</v>
+        <v>32.57876834436517</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1703009161402403</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="17">
@@ -26041,37 +26041,37 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>5.307383521924541</v>
+        <v>5.329914737938587</v>
       </c>
       <c r="D17" t="n">
-        <v>0.44487055515683</v>
+        <v>0.4467597970114416</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4624857984125063</v>
+        <v>0.4644498266902296</v>
       </c>
       <c r="F17" t="n">
-        <v>5.352930045018794</v>
+        <v>5.352933937622248</v>
       </c>
       <c r="G17" t="n">
-        <v>67.89409842533405</v>
+        <v>67.89414779732283</v>
       </c>
       <c r="H17" t="n">
-        <v>1.221847113761313</v>
+        <v>1.231950270350026</v>
       </c>
       <c r="I17" t="n">
-        <v>0.7716584514413147</v>
+        <v>0.778040241671801</v>
       </c>
       <c r="J17" t="n">
-        <v>9.842944253416565</v>
+        <v>9.884722470912312</v>
       </c>
       <c r="K17" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.0518514430121362</v>
       </c>
       <c r="L17" t="n">
-        <v>32.46546047174457</v>
+        <v>32.87169140609178</v>
       </c>
       <c r="M17" t="n">
-        <v>0.1703009161402404</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="18">
@@ -26082,37 +26082,37 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>5.321899138109929</v>
+        <v>5.344491975442158</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4448938876653625</v>
+        <v>0.4467832285040458</v>
       </c>
       <c r="E18" t="n">
-        <v>0.4624857984125063</v>
+        <v>0.4644498266902298</v>
       </c>
       <c r="F18" t="n">
-        <v>5.357711999348352</v>
+        <v>5.3577158954292</v>
       </c>
       <c r="G18" t="n">
-        <v>67.95475053085123</v>
+        <v>67.95479994694566</v>
       </c>
       <c r="H18" t="n">
-        <v>1.224031123953894</v>
+        <v>1.234152339591664</v>
       </c>
       <c r="I18" t="n">
-        <v>0.771658451441315</v>
+        <v>0.7780402416718011</v>
       </c>
       <c r="J18" t="n">
-        <v>9.860538181766811</v>
+        <v>9.902391076406541</v>
       </c>
       <c r="K18" t="n">
-        <v>0.05163217769028857</v>
+        <v>0.05185144301213621</v>
       </c>
       <c r="L18" t="n">
-        <v>32.52349137903122</v>
+        <v>32.93044843736821</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1703009161402404</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="19">
@@ -26123,37 +26123,37 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>5.424200793687952</v>
+        <v>5.44722792653373</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4450562847917333</v>
+        <v>0.4469463151665373</v>
       </c>
       <c r="E19" t="n">
-        <v>0.4624857984125062</v>
+        <v>0.4644498266902297</v>
       </c>
       <c r="F19" t="n">
-        <v>5.391168482525194</v>
+        <v>5.391172402935302</v>
       </c>
       <c r="G19" t="n">
-        <v>68.37909714899689</v>
+        <v>68.37914687367244</v>
       </c>
       <c r="H19" t="n">
-        <v>1.239365893480153</v>
+        <v>1.249613908597195</v>
       </c>
       <c r="I19" t="n">
-        <v>0.771658451441315</v>
+        <v>0.7780402416718007</v>
       </c>
       <c r="J19" t="n">
-        <v>9.984071870954249</v>
+        <v>10.02644910233734</v>
       </c>
       <c r="K19" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.05185144301213621</v>
       </c>
       <c r="L19" t="n">
-        <v>32.93094853818879</v>
+        <v>33.34300399032849</v>
       </c>
       <c r="M19" t="n">
-        <v>0.1703009161402403</v>
+        <v>0.1724322193841203</v>
       </c>
     </row>
     <row r="20">
@@ -26164,37 +26164,37 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>5.617060904988275</v>
+        <v>5.640906749006453</v>
       </c>
       <c r="D20" t="n">
-        <v>0.445325389232243</v>
+        <v>0.4472165600566776</v>
       </c>
       <c r="E20" t="n">
-        <v>0.4624857984125062</v>
+        <v>0.4644498266902296</v>
       </c>
       <c r="F20" t="n">
-        <v>5.453222150533805</v>
+        <v>5.453226116068792</v>
       </c>
       <c r="G20" t="n">
-        <v>69.16615728391312</v>
+        <v>69.16620758093185</v>
       </c>
       <c r="H20" t="n">
-        <v>1.268060900986079</v>
+        <v>1.278546188140581</v>
       </c>
       <c r="I20" t="n">
-        <v>0.7716584514413148</v>
+        <v>0.7780402416718011</v>
       </c>
       <c r="J20" t="n">
-        <v>10.21523283704495</v>
+        <v>10.25859122740539</v>
       </c>
       <c r="K20" t="n">
-        <v>0.05163217769028854</v>
+        <v>0.05185144301213619</v>
       </c>
       <c r="L20" t="n">
-        <v>33.69339796531248</v>
+        <v>34.11499372702033</v>
       </c>
       <c r="M20" t="n">
-        <v>0.1703009161402403</v>
+        <v>0.1724322193841203</v>
       </c>
     </row>
     <row r="21">
@@ -26205,37 +26205,37 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>5.906058321495612</v>
+        <v>5.931131002932267</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4456762792120866</v>
+        <v>0.4475689379258621</v>
       </c>
       <c r="E21" t="n">
-        <v>0.4624857984125062</v>
+        <v>0.4644498266902297</v>
       </c>
       <c r="F21" t="n">
-        <v>5.543729548969965</v>
+        <v>5.543733580321133</v>
       </c>
       <c r="G21" t="n">
-        <v>70.31411142603081</v>
+        <v>70.31416255783165</v>
       </c>
       <c r="H21" t="n">
-        <v>1.310502342951277</v>
+        <v>1.321338568066181</v>
       </c>
       <c r="I21" t="n">
-        <v>0.7716584514413148</v>
+        <v>0.7780402416718012</v>
       </c>
       <c r="J21" t="n">
-        <v>10.55713219793313</v>
+        <v>10.60194177459446</v>
       </c>
       <c r="K21" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.0518514430121362</v>
       </c>
       <c r="L21" t="n">
-        <v>34.82110121146032</v>
+        <v>35.25680759832773</v>
       </c>
       <c r="M21" t="n">
-        <v>0.1703009161402404</v>
+        <v>0.1724322193841203</v>
       </c>
     </row>
     <row r="22">
@@ -26246,37 +26246,37 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>6.299199980372795</v>
+        <v>6.325941616104705</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4460596240665165</v>
+        <v>0.4479539086471665</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4624857984125064</v>
+        <v>0.4644498266902297</v>
       </c>
       <c r="F22" t="n">
-        <v>5.662481444675715</v>
+        <v>5.662485562382211</v>
       </c>
       <c r="G22" t="n">
-        <v>71.82030575837481</v>
+        <v>71.82035798546684</v>
       </c>
       <c r="H22" t="n">
-        <v>1.367248058679943</v>
+        <v>1.378553500315709</v>
       </c>
       <c r="I22" t="n">
-        <v>0.7716584514413148</v>
+        <v>0.7780402416718007</v>
       </c>
       <c r="J22" t="n">
-        <v>11.01426379013215</v>
+        <v>11.06101365443418</v>
       </c>
       <c r="K22" t="n">
-        <v>0.05163217769028857</v>
+        <v>0.05185144301213623</v>
       </c>
       <c r="L22" t="n">
-        <v>36.32888051558179</v>
+        <v>36.78345330959704</v>
       </c>
       <c r="M22" t="n">
-        <v>0.1703009161402404</v>
+        <v>0.1724322193841203</v>
       </c>
     </row>
     <row r="23">
@@ -26287,37 +26287,37 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>6.807270747818999</v>
+        <v>6.836169228419143</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4464277572173123</v>
+        <v>0.4483236025880508</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4624857984125062</v>
+        <v>0.4644498266902297</v>
       </c>
       <c r="F23" t="n">
-        <v>5.809203309440319</v>
+        <v>5.80920753384166</v>
       </c>
       <c r="G23" t="n">
-        <v>73.68125829160404</v>
+        <v>73.68131187196434</v>
       </c>
       <c r="H23" t="n">
-        <v>1.439020178515435</v>
+        <v>1.450919086352687</v>
       </c>
       <c r="I23" t="n">
-        <v>0.7716584514413148</v>
+        <v>0.7780402416718007</v>
       </c>
       <c r="J23" t="n">
-        <v>11.592444944332</v>
+        <v>11.64164888918048</v>
       </c>
       <c r="K23" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.0518514430121362</v>
       </c>
       <c r="L23" t="n">
-        <v>38.23592346166649</v>
+        <v>38.71435853351705</v>
       </c>
       <c r="M23" t="n">
-        <v>0.1703009161402404</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="24">
@@ -26328,37 +26328,37 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>7.444038205006621</v>
+        <v>7.475639869722505</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4467436797068086</v>
+        <v>0.4486408640095963</v>
       </c>
       <c r="E24" t="n">
-        <v>0.4624857984125064</v>
+        <v>0.4644498266902296</v>
       </c>
       <c r="F24" t="n">
-        <v>5.983555954648961</v>
+        <v>5.983560305838005</v>
       </c>
       <c r="G24" t="n">
-        <v>75.89266691360319</v>
+        <v>75.8927221020803</v>
       </c>
       <c r="H24" t="n">
-        <v>1.526695568299473</v>
+        <v>1.539319442609198</v>
       </c>
       <c r="I24" t="n">
-        <v>0.771658451441315</v>
+        <v>0.7780402416718006</v>
       </c>
       <c r="J24" t="n">
-        <v>12.29873950796546</v>
+        <v>12.35094130865218</v>
       </c>
       <c r="K24" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.0518514430121362</v>
       </c>
       <c r="L24" t="n">
-        <v>40.56552908034008</v>
+        <v>41.07311383475739</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1703009161402403</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="25">
@@ -26369,37 +26369,37 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>8.217596766490637</v>
+        <v>8.252481931849404</v>
       </c>
       <c r="D25" t="n">
-        <v>0.4465035269207772</v>
+        <v>0.4483996677619224</v>
       </c>
       <c r="E25" t="n">
-        <v>0.462485798412506</v>
+        <v>0.4644498266902297</v>
       </c>
       <c r="F25" t="n">
-        <v>6.185136315412086</v>
+        <v>6.18514081318859</v>
       </c>
       <c r="G25" t="n">
-        <v>78.44941933501801</v>
+        <v>78.44947638274293</v>
       </c>
       <c r="H25" t="n">
-        <v>1.631294165048162</v>
+        <v>1.644782939712448</v>
       </c>
       <c r="I25" t="n">
-        <v>0.7716584514413146</v>
+        <v>0.7780402416718007</v>
       </c>
       <c r="J25" t="n">
-        <v>13.14136387985891</v>
+        <v>13.19714218604743</v>
       </c>
       <c r="K25" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.05185144301213622</v>
       </c>
       <c r="L25" t="n">
-        <v>43.3447979183953</v>
+        <v>43.88715886142906</v>
       </c>
       <c r="M25" t="n">
-        <v>0.1703009161402403</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="26">
@@ -26410,37 +26410,37 @@
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>9.14486151058199</v>
+        <v>9.183683111929948</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4456810009909744</v>
+        <v>0.4475736503989255</v>
       </c>
       <c r="E26" t="n">
-        <v>0.4624857984125063</v>
+        <v>0.4644498266902298</v>
       </c>
       <c r="F26" t="n">
-        <v>6.413478382362587</v>
+        <v>6.413483046187425</v>
       </c>
       <c r="G26" t="n">
-        <v>81.34560490774152</v>
+        <v>81.34566406154698</v>
       </c>
       <c r="H26" t="n">
-        <v>1.753965319875023</v>
+        <v>1.768468432480755</v>
       </c>
       <c r="I26" t="n">
-        <v>0.7716584514413147</v>
+        <v>0.7780402416718007</v>
       </c>
       <c r="J26" t="n">
-        <v>14.12957699168274</v>
+        <v>14.18954975242215</v>
       </c>
       <c r="K26" t="n">
-        <v>0.05163217769028857</v>
+        <v>0.05185144301213622</v>
       </c>
       <c r="L26" t="n">
-        <v>46.60426915927325</v>
+        <v>47.18741492495914</v>
       </c>
       <c r="M26" t="n">
-        <v>0.1703009161402404</v>
+        <v>0.1724322193841203</v>
       </c>
     </row>
     <row r="27">
@@ -26451,37 +26451,37 @@
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>10.25928975059792</v>
+        <v>10.30284233522691</v>
       </c>
       <c r="D27" t="n">
-        <v>0.444885048161714</v>
+        <v>0.4467743188531483</v>
       </c>
       <c r="E27" t="n">
-        <v>0.4624857984125063</v>
+        <v>0.4644498266902296</v>
       </c>
       <c r="F27" t="n">
-        <v>6.668054278966745</v>
+        <v>6.668059127916925</v>
       </c>
       <c r="G27" t="n">
-        <v>84.57452828902953</v>
+        <v>84.57458979087954</v>
       </c>
       <c r="H27" t="n">
-        <v>1.895972284157914</v>
+        <v>1.911649617810354</v>
       </c>
       <c r="I27" t="n">
-        <v>0.771658451441315</v>
+        <v>0.7780402416718009</v>
       </c>
       <c r="J27" t="n">
-        <v>15.27355533176373</v>
+        <v>15.33838369004304</v>
       </c>
       <c r="K27" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.05185144301213621</v>
       </c>
       <c r="L27" t="n">
-        <v>50.37750840804171</v>
+        <v>51.00786762714146</v>
       </c>
       <c r="M27" t="n">
-        <v>0.1703009161402404</v>
+        <v>0.1724322193841202</v>
       </c>
     </row>
     <row r="28">
@@ -26492,37 +26492,37 @@
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>11.58795871655964</v>
+        <v>11.63715177747461</v>
       </c>
       <c r="D28" t="n">
-        <v>0.4441234926127889</v>
+        <v>0.4460095304141994</v>
       </c>
       <c r="E28" t="n">
-        <v>0.4624857984125063</v>
+        <v>0.4644498266902297</v>
       </c>
       <c r="F28" t="n">
-        <v>6.94827548185845</v>
+        <v>6.948280534583016</v>
       </c>
       <c r="G28" t="n">
-        <v>88.12872491965787</v>
+        <v>88.1287890060883</v>
       </c>
       <c r="H28" t="n">
-        <v>2.058674993633933</v>
+        <v>2.075697676416171</v>
       </c>
       <c r="I28" t="n">
-        <v>0.7716584514413146</v>
+        <v>0.7780402416718009</v>
       </c>
       <c r="J28" t="n">
-        <v>16.58425425736198</v>
+        <v>16.65464585600671</v>
       </c>
       <c r="K28" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.05185144301213621</v>
       </c>
       <c r="L28" t="n">
-        <v>54.70065025095096</v>
+        <v>55.38510369587232</v>
       </c>
       <c r="M28" t="n">
-        <v>0.1703009161402404</v>
+        <v>0.1724322193841203</v>
       </c>
     </row>
     <row r="29">
@@ -26533,78 +26533,78 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>13.16116196506577</v>
+        <v>13.21703359347101</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4433843157151465</v>
+        <v>0.4452672153070044</v>
       </c>
       <c r="E29" t="n">
-        <v>0.4624857984125063</v>
+        <v>0.4644498266902296</v>
       </c>
       <c r="F29" t="n">
-        <v>7.253494181375511</v>
+        <v>7.25349945605242</v>
       </c>
       <c r="G29" t="n">
-        <v>91.99997828033784</v>
+        <v>92.00004518190954</v>
       </c>
       <c r="H29" t="n">
-        <v>2.243511322337868</v>
+        <v>2.262062371763645</v>
       </c>
       <c r="I29" t="n">
-        <v>0.7716584514413147</v>
+        <v>0.778040241671801</v>
       </c>
       <c r="J29" t="n">
-        <v>18.07325698032821</v>
+        <v>18.14996862691896</v>
       </c>
       <c r="K29" t="n">
-        <v>0.05163217769028856</v>
+        <v>0.05185144301213618</v>
       </c>
       <c r="L29" t="n">
-        <v>59.61190015750204</v>
+        <v>60.35780665466296</v>
       </c>
       <c r="M29" t="n">
-        <v>0.1703009161402403</v>
+        <v>0.1724322193841203</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>10.66821594497437</v>
+        <v>10.65319618433997</v>
       </c>
       <c r="B30" t="n">
-        <v>1.463672932855431e-18</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>15</v>
       </c>
       <c r="D30" t="n">
-        <v>0.4429291208253771</v>
+        <v>0.4448058509240232</v>
       </c>
       <c r="E30" t="n">
-        <v>0.4625586844088074</v>
+        <v>0.4645185975221373</v>
       </c>
       <c r="F30" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G30" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H30" t="n">
-        <v>2.426962624026543</v>
+        <v>2.443067125507037</v>
       </c>
       <c r="I30" t="n">
-        <v>0.7645358611520446</v>
+        <v>0.7717818344287677</v>
       </c>
       <c r="J30" t="n">
-        <v>19.94700250291289</v>
+        <v>19.94698865675457</v>
       </c>
       <c r="K30" t="n">
-        <v>0.05219147642648304</v>
+        <v>0.05233882604080675</v>
       </c>
       <c r="L30" t="n">
-        <v>64.44308440374573</v>
+        <v>65.14934831142496</v>
       </c>
       <c r="M30" t="n">
-        <v>0.1686157967853462</v>
+        <v>0.1709451219239019</v>
       </c>
     </row>
     <row r="31">
@@ -26612,40 +26612,40 @@
         <v>10.67345003876854</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.660569642234772</v>
+        <v>0.6841171437409598</v>
       </c>
       <c r="C31" t="n">
-        <v>14.99999002936336</v>
+        <v>15.00003275832904</v>
       </c>
       <c r="D31" t="n">
-        <v>0.4422775293613888</v>
+        <v>0.4422794339664348</v>
       </c>
       <c r="E31" t="n">
-        <v>0.4618782159632177</v>
+        <v>0.4618802157214996</v>
       </c>
       <c r="F31" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G31" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H31" t="n">
-        <v>2.522062020985371</v>
+        <v>2.345793945866424</v>
       </c>
       <c r="I31" t="n">
-        <v>0.7937148180362047</v>
+        <v>0.7382428003674041</v>
       </c>
       <c r="J31" t="n">
-        <v>19.94698922930437</v>
+        <v>19.94703200905402</v>
       </c>
       <c r="K31" t="n">
-        <v>0.05214026650526233</v>
+        <v>0.0521404923408025</v>
       </c>
       <c r="L31" t="n">
-        <v>67.14396379530938</v>
+        <v>62.36636251971841</v>
       </c>
       <c r="M31" t="n">
-        <v>0.1755104054181717</v>
+        <v>0.1630223907901227</v>
       </c>
     </row>
     <row r="32">
@@ -26653,40 +26653,40 @@
         <v>11.17037214438025</v>
       </c>
       <c r="B32" t="n">
-        <v>3.684874514101414</v>
+        <v>3.775833125022726</v>
       </c>
       <c r="C32" t="n">
-        <v>15.00000016996025</v>
+        <v>14.9999999821673</v>
       </c>
       <c r="D32" t="n">
-        <v>0.385839518622599</v>
+        <v>0.3858400762509693</v>
       </c>
       <c r="E32" t="n">
-        <v>0.4029390070231109</v>
+        <v>0.4029395987386614</v>
       </c>
       <c r="F32" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G32" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H32" t="n">
-        <v>1.947971521416511</v>
+        <v>1.946230667815811</v>
       </c>
       <c r="I32" t="n">
-        <v>0.5597133794982958</v>
+        <v>0.5592139927953637</v>
       </c>
       <c r="J32" t="n">
-        <v>19.94700271427181</v>
+        <v>19.94698842333938</v>
       </c>
       <c r="K32" t="n">
-        <v>0.04760448808383468</v>
+        <v>0.04760455807120892</v>
       </c>
       <c r="L32" t="n">
-        <v>50.55642232233696</v>
+        <v>50.6798849153516</v>
       </c>
       <c r="M32" t="n">
-        <v>0.1206553505045163</v>
+        <v>0.1209502644355143</v>
       </c>
     </row>
     <row r="33">
@@ -26694,40 +26694,40 @@
         <v>11.69926530163598</v>
       </c>
       <c r="B33" t="n">
-        <v>5.355006777463386</v>
+        <v>5.423082088342932</v>
       </c>
       <c r="C33" t="n">
-        <v>14.99999999780361</v>
+        <v>14.9999999983679</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3358411123480712</v>
+        <v>0.3358416019342602</v>
       </c>
       <c r="E33" t="n">
-        <v>0.3507247904780659</v>
+        <v>0.3507253099211985</v>
       </c>
       <c r="F33" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G33" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H33" t="n">
-        <v>1.762601872445613</v>
+        <v>1.76205727092549</v>
       </c>
       <c r="I33" t="n">
-        <v>0.4616952615225133</v>
+        <v>0.4615532816381845</v>
       </c>
       <c r="J33" t="n">
-        <v>19.94700248533788</v>
+        <v>19.94698844488292</v>
       </c>
       <c r="K33" t="n">
-        <v>0.04339762866149547</v>
+        <v>0.04339769300896202</v>
       </c>
       <c r="L33" t="n">
-        <v>44.95548533226845</v>
+        <v>45.08539610064135</v>
       </c>
       <c r="M33" t="n">
-        <v>0.0978072499956399</v>
+        <v>0.09809010440696481</v>
       </c>
     </row>
     <row r="34">
@@ -26735,40 +26735,40 @@
         <v>12.2589068261207</v>
       </c>
       <c r="B34" t="n">
-        <v>6.721863874678244</v>
+        <v>6.776145393658523</v>
       </c>
       <c r="C34" t="n">
-        <v>14.9999922478468</v>
+        <v>14.99999141577645</v>
       </c>
       <c r="D34" t="n">
-        <v>0.2919134939933235</v>
+        <v>0.2919139033383699</v>
       </c>
       <c r="E34" t="n">
-        <v>0.3048504047128657</v>
+        <v>0.3048508392914865</v>
       </c>
       <c r="F34" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G34" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H34" t="n">
-        <v>1.625902295299744</v>
+        <v>1.62580083705044</v>
       </c>
       <c r="I34" t="n">
-        <v>0.3878906622565633</v>
+        <v>0.3878670228286475</v>
       </c>
       <c r="J34" t="n">
-        <v>19.94699217944403</v>
+        <v>19.94697703175942</v>
       </c>
       <c r="K34" t="n">
-        <v>0.03952569049371831</v>
+        <v>0.03952574690606633</v>
       </c>
       <c r="L34" t="n">
-        <v>40.71093239369927</v>
+        <v>40.83079400623923</v>
       </c>
       <c r="M34" t="n">
-        <v>0.08067019323155408</v>
+        <v>0.08090788029157273</v>
       </c>
     </row>
     <row r="35">
@@ -26776,40 +26776,40 @@
         <v>12.84800294997107</v>
       </c>
       <c r="B35" t="n">
-        <v>7.942244744069674</v>
+        <v>7.986108290484959</v>
       </c>
       <c r="C35" t="n">
-        <v>14.99999988258478</v>
+        <v>14.99999986537553</v>
       </c>
       <c r="D35" t="n">
-        <v>0.2535728441477668</v>
+        <v>0.2535732135035461</v>
       </c>
       <c r="E35" t="n">
-        <v>0.2648105885930958</v>
+        <v>0.2648109804786902</v>
       </c>
       <c r="F35" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G35" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H35" t="n">
-        <v>1.514904678202373</v>
+        <v>1.515042910591406</v>
       </c>
       <c r="I35" t="n">
-        <v>0.3290276689009596</v>
+        <v>0.3290581717823925</v>
       </c>
       <c r="J35" t="n">
-        <v>19.94700233211985</v>
+        <v>19.94698826802977</v>
       </c>
       <c r="K35" t="n">
-        <v>0.03598420561891255</v>
+        <v>0.03598425893155102</v>
       </c>
       <c r="L35" t="n">
-        <v>37.17475153187447</v>
+        <v>37.28141956572362</v>
       </c>
       <c r="M35" t="n">
-        <v>0.06706290402347347</v>
+        <v>0.06725547922134009</v>
       </c>
     </row>
     <row r="36">
@@ -26817,40 +26817,40 @@
         <v>13.46519181278163</v>
       </c>
       <c r="B36" t="n">
-        <v>9.07533324981449</v>
+        <v>9.110537854821954</v>
       </c>
       <c r="C36" t="n">
-        <v>14.99999999433258</v>
+        <v>14.99999999363886</v>
       </c>
       <c r="D36" t="n">
-        <v>0.2202784414215901</v>
+        <v>0.2202787625230705</v>
       </c>
       <c r="E36" t="n">
-        <v>0.2300406572449402</v>
+        <v>0.2300409979287939</v>
       </c>
       <c r="F36" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G36" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H36" t="n">
-        <v>1.420738604789053</v>
+        <v>1.421038908269891</v>
       </c>
       <c r="I36" t="n">
-        <v>0.2809360435080113</v>
+        <v>0.2809958349695443</v>
       </c>
       <c r="J36" t="n">
-        <v>19.94700248072209</v>
+        <v>19.94698843859425</v>
       </c>
       <c r="K36" t="n">
-        <v>0.03276107089487181</v>
+        <v>0.03276111946832481</v>
       </c>
       <c r="L36" t="n">
-        <v>34.09775794014271</v>
+        <v>34.19084512237261</v>
       </c>
       <c r="M36" t="n">
-        <v>0.05600235254960246</v>
+        <v>0.05615536226058895</v>
       </c>
     </row>
     <row r="37">
@@ -26858,40 +26858,40 @@
         <v>14.10904660992588</v>
       </c>
       <c r="B37" t="n">
-        <v>10.15041350007385</v>
+        <v>10.17802968738675</v>
       </c>
       <c r="C37" t="n">
-        <v>14.9999211560002</v>
+        <v>14.99992662064703</v>
       </c>
       <c r="D37" t="n">
-        <v>0.1914759975908077</v>
+        <v>0.1914763464726608</v>
       </c>
       <c r="E37" t="n">
-        <v>0.1999617577106335</v>
+        <v>0.1999621267062328</v>
       </c>
       <c r="F37" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G37" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H37" t="n">
-        <v>1.338858919641432</v>
+        <v>1.339289019918691</v>
       </c>
       <c r="I37" t="n">
-        <v>0.241133666099282</v>
+        <v>0.241211480447914</v>
       </c>
       <c r="J37" t="n">
-        <v>19.94689764149463</v>
+        <v>19.94689086724622</v>
       </c>
       <c r="K37" t="n">
-        <v>0.02983908896401134</v>
+        <v>0.02983914407729084</v>
       </c>
       <c r="L37" t="n">
-        <v>31.35314031573148</v>
+        <v>31.4331265432092</v>
       </c>
       <c r="M37" t="n">
-        <v>0.04690198746676583</v>
+        <v>0.04702174378778369</v>
       </c>
     </row>
     <row r="38">
@@ -26899,40 +26899,40 @@
         <v>14.77807889101415</v>
       </c>
       <c r="B38" t="n">
-        <v>11.18388860574722</v>
+        <v>11.2046541576123</v>
       </c>
       <c r="C38" t="n">
-        <v>15.00006167341835</v>
+        <v>15.00006437360995</v>
       </c>
       <c r="D38" t="n">
-        <v>0.1666316412082445</v>
+        <v>0.1666319141118459</v>
       </c>
       <c r="E38" t="n">
-        <v>0.174016358632137</v>
+        <v>0.1740166476786861</v>
       </c>
       <c r="F38" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G38" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H38" t="n">
-        <v>1.266593650789173</v>
+        <v>1.267138333784447</v>
       </c>
       <c r="I38" t="n">
-        <v>0.2079312261077572</v>
+        <v>0.2080209476126837</v>
       </c>
       <c r="J38" t="n">
-        <v>19.94708450158059</v>
+        <v>19.94707405103022</v>
       </c>
       <c r="K38" t="n">
-        <v>0.02719875360356439</v>
+        <v>0.02719879882737307</v>
       </c>
       <c r="L38" t="n">
-        <v>28.86700987022205</v>
+        <v>28.93457283617217</v>
       </c>
       <c r="M38" t="n">
-        <v>0.03936147604275784</v>
+        <v>0.03945368747885979</v>
       </c>
     </row>
     <row r="39">
@@ -26940,40 +26940,40 @@
         <v>15.47074200086285</v>
       </c>
       <c r="B39" t="n">
-        <v>12.18603087349094</v>
+        <v>12.20050327245719</v>
       </c>
       <c r="C39" t="n">
-        <v>15.00003054205507</v>
+        <v>15.00003142036035</v>
       </c>
       <c r="D39" t="n">
-        <v>0.14523693711894</v>
+        <v>0.1452371573427455</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1516734922195085</v>
+        <v>0.1516737257318088</v>
       </c>
       <c r="F39" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G39" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H39" t="n">
-        <v>1.202139420728024</v>
+        <v>1.202791822527804</v>
       </c>
       <c r="I39" t="n">
-        <v>0.180073962266577</v>
+        <v>0.1801719511620791</v>
       </c>
       <c r="J39" t="n">
-        <v>19.94704310308854</v>
+        <v>19.94703022982428</v>
       </c>
       <c r="K39" t="n">
-        <v>0.02481771399960557</v>
+        <v>0.02481775225009511</v>
       </c>
       <c r="L39" t="n">
-        <v>26.59001748451232</v>
+        <v>26.64578279922473</v>
       </c>
       <c r="M39" t="n">
-        <v>0.0330827705021082</v>
+        <v>0.03315222508823713</v>
       </c>
     </row>
     <row r="40">
@@ -26981,40 +26981,40 @@
         <v>16.18543465502034</v>
       </c>
       <c r="B40" t="n">
-        <v>13.16322614708007</v>
+        <v>13.17187359405491</v>
       </c>
       <c r="C40" t="n">
-        <v>15.00001707594489</v>
+        <v>15.00001738053231</v>
       </c>
       <c r="D40" t="n">
-        <v>0.1268343893635816</v>
+        <v>0.1268345768323341</v>
       </c>
       <c r="E40" t="n">
-        <v>0.1324553873822681</v>
+        <v>0.132455586240778</v>
       </c>
       <c r="F40" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G40" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H40" t="n">
-        <v>1.144268060387364</v>
+        <v>1.14502393074655</v>
       </c>
       <c r="I40" t="n">
-        <v>0.1566020386540157</v>
+        <v>0.1567057138657822</v>
       </c>
       <c r="J40" t="n">
-        <v>19.94702519585298</v>
+        <v>19.94701155967178</v>
       </c>
       <c r="K40" t="n">
-        <v>0.02267435486773002</v>
+        <v>0.0226743889475065</v>
       </c>
       <c r="L40" t="n">
-        <v>24.48899852592321</v>
+        <v>24.533395281931</v>
       </c>
       <c r="M40" t="n">
-        <v>0.02783734604433858</v>
+        <v>0.02788787408887317</v>
       </c>
     </row>
     <row r="41">
@@ -27022,40 +27022,40 @@
         <v>16.92050464158374</v>
       </c>
       <c r="B41" t="n">
-        <v>14.11972063558667</v>
+        <v>14.1229503856142</v>
       </c>
       <c r="C41" t="n">
-        <v>15.00001046848861</v>
+        <v>15.00001055936076</v>
       </c>
       <c r="D41" t="n">
-        <v>0.111012017907811</v>
+        <v>0.1110121804084952</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1159318061122659</v>
+        <v>0.1159319785117594</v>
       </c>
       <c r="F41" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G41" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H41" t="n">
-        <v>1.092052136541136</v>
+        <v>1.092907232284398</v>
       </c>
       <c r="I41" t="n">
-        <v>0.1367524510937358</v>
+        <v>0.1368597301397058</v>
       </c>
       <c r="J41" t="n">
-        <v>19.94701640925653</v>
+        <v>19.94700248888309</v>
       </c>
       <c r="K41" t="n">
-        <v>0.02074707412999461</v>
+        <v>0.02074710501745151</v>
       </c>
       <c r="L41" t="n">
-        <v>22.53928026379342</v>
+        <v>22.57255923402057</v>
       </c>
       <c r="M41" t="n">
-        <v>0.02344331146449766</v>
+        <v>0.02347797656323912</v>
       </c>
     </row>
     <row r="42">
@@ -27063,40 +27063,40 @@
         <v>17.67425264074866</v>
       </c>
       <c r="B42" t="n">
-        <v>15.05833296569638</v>
+        <v>15.05650234622196</v>
       </c>
       <c r="C42" t="n">
-        <v>15.00000685196746</v>
+        <v>15.00000688390757</v>
       </c>
       <c r="D42" t="n">
-        <v>0.09740621113891453</v>
+        <v>0.09740635334057042</v>
       </c>
       <c r="E42" t="n">
-        <v>0.1017230223962312</v>
+        <v>0.1017231732665228</v>
       </c>
       <c r="F42" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G42" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H42" t="n">
-        <v>1.04476845080427</v>
+        <v>1.045720600819485</v>
       </c>
       <c r="I42" t="n">
-        <v>0.1199102480801606</v>
+        <v>0.1200197032766408</v>
       </c>
       <c r="J42" t="n">
-        <v>19.94701160000611</v>
+        <v>19.94699760126828</v>
       </c>
       <c r="K42" t="n">
-        <v>0.01901521584585163</v>
+        <v>0.01901524408027655</v>
       </c>
       <c r="L42" t="n">
-        <v>20.72190702130683</v>
+        <v>20.74421621125506</v>
       </c>
       <c r="M42" t="n">
-        <v>0.01975391314996264</v>
+        <v>0.01977522343943953</v>
       </c>
     </row>
     <row r="43">
@@ -27104,40 +27104,40 @@
         <v>18.44493615326207</v>
       </c>
       <c r="B43" t="n">
-        <v>15.98091465799603</v>
+        <v>15.97432316229584</v>
       </c>
       <c r="C43" t="n">
-        <v>15.00000468071182</v>
+        <v>15.00000472431107</v>
       </c>
       <c r="D43" t="n">
-        <v>0.08569950134432436</v>
+        <v>0.08569962652216775</v>
       </c>
       <c r="E43" t="n">
-        <v>0.08949749910877909</v>
+        <v>0.08949763191637529</v>
       </c>
       <c r="F43" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G43" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H43" t="n">
-        <v>1.001834367896723</v>
+        <v>1.002884012918521</v>
       </c>
       <c r="I43" t="n">
-        <v>0.1055747307918257</v>
+        <v>0.1056854979405153</v>
       </c>
       <c r="J43" t="n">
-        <v>19.94700871267</v>
+        <v>19.94699472943851</v>
       </c>
       <c r="K43" t="n">
-        <v>0.01745938739707859</v>
+        <v>0.01745941333492846</v>
       </c>
       <c r="L43" t="n">
-        <v>19.02179063525498</v>
+        <v>19.03329877186704</v>
       </c>
       <c r="M43" t="n">
-        <v>0.0166495546510735</v>
+        <v>0.01665966401920071</v>
       </c>
     </row>
     <row r="44">
@@ -27145,40 +27145,40 @@
         <v>19.23077352869659</v>
       </c>
       <c r="B44" t="n">
-        <v>16.88862132100929</v>
+        <v>16.87750674524488</v>
       </c>
       <c r="C44" t="n">
-        <v>15.00000325919399</v>
+        <v>15.00000330560118</v>
       </c>
       <c r="D44" t="n">
-        <v>0.07561700329840436</v>
+        <v>0.0756171137633003</v>
       </c>
       <c r="E44" t="n">
-        <v>0.07896816876584645</v>
+        <v>0.07896828596348639</v>
       </c>
       <c r="F44" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G44" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H44" t="n">
-        <v>0.962770058243146</v>
+        <v>0.9639193696721043</v>
       </c>
       <c r="I44" t="n">
-        <v>0.09333562451547042</v>
+        <v>0.09344718059291093</v>
       </c>
       <c r="J44" t="n">
-        <v>19.94700682233534</v>
+        <v>19.94699284283919</v>
       </c>
       <c r="K44" t="n">
-        <v>0.01606163550196763</v>
+        <v>0.01606165936630925</v>
       </c>
       <c r="L44" t="n">
-        <v>17.4266523354435</v>
+        <v>17.4276334915197</v>
       </c>
       <c r="M44" t="n">
-        <v>0.01403220745470404</v>
+        <v>0.0140330281815968</v>
       </c>
     </row>
     <row r="45">
@@ -27186,40 +27186,40 @@
         <v>20.02994808423354</v>
       </c>
       <c r="B45" t="n">
-        <v>17.78209885106097</v>
+        <v>17.76665857318871</v>
       </c>
       <c r="C45" t="n">
-        <v>15.00000226528597</v>
+        <v>15.00000230863784</v>
       </c>
       <c r="D45" t="n">
-        <v>0.06692220205416509</v>
+        <v>0.06692229980365275</v>
       </c>
       <c r="E45" t="n">
-        <v>0.06988803464136882</v>
+        <v>0.06988813834883358</v>
       </c>
       <c r="F45" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G45" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H45" t="n">
-        <v>0.9271744470980213</v>
+        <v>0.9284250292018574</v>
       </c>
       <c r="I45" t="n">
-        <v>0.08285527742963149</v>
+        <v>0.08296715439630997</v>
       </c>
       <c r="J45" t="n">
-        <v>19.9470055006363</v>
+        <v>19.94699151707812</v>
       </c>
       <c r="K45" t="n">
-        <v>0.01480551766205247</v>
+        <v>0.01480553965704134</v>
       </c>
       <c r="L45" t="n">
-        <v>15.92631870374659</v>
+        <v>15.91709294337797</v>
       </c>
       <c r="M45" t="n">
-        <v>0.01182119255204872</v>
+        <v>0.01181437063309664</v>
       </c>
     </row>
     <row r="46">
@@ -27227,40 +27227,40 @@
         <v>20.8406123044333</v>
       </c>
       <c r="B46" t="n">
-        <v>18.66160622438338</v>
+        <v>18.64202027396687</v>
       </c>
       <c r="C46" t="n">
-        <v>15.00000153416181</v>
+        <v>15.00000157281846</v>
       </c>
       <c r="D46" t="n">
-        <v>0.05941255768924885</v>
+        <v>0.05941264445122531</v>
       </c>
       <c r="E46" t="n">
-        <v>0.06204558072607717</v>
+        <v>0.06204567277663486</v>
       </c>
       <c r="F46" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G46" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H46" t="n">
-        <v>0.8947073085418855</v>
+        <v>0.8960568601788775</v>
       </c>
       <c r="I46" t="n">
-        <v>0.07385474534630777</v>
+        <v>0.07396625361590013</v>
       </c>
       <c r="J46" t="n">
-        <v>19.94700452838728</v>
+        <v>19.94699053858606</v>
       </c>
       <c r="K46" t="n">
-        <v>0.01367610019068536</v>
+        <v>0.01367612050353753</v>
       </c>
       <c r="L46" t="n">
-        <v>14.51226253133243</v>
+        <v>14.49310245714383</v>
       </c>
       <c r="M46" t="n">
-        <v>0.009949922861328892</v>
+        <v>0.009936808025781762</v>
       </c>
     </row>
     <row r="47">
@@ -27268,40 +27268,40 @@
         <v>21.66089211228376</v>
       </c>
       <c r="B47" t="n">
-        <v>19.52712097550045</v>
+        <v>19.50356243150797</v>
       </c>
       <c r="C47" t="n">
-        <v>15.00000098310709</v>
+        <v>15.00000102194977</v>
       </c>
       <c r="D47" t="n">
-        <v>0.05291522400094138</v>
+        <v>0.05291530127531888</v>
       </c>
       <c r="E47" t="n">
-        <v>0.05526030068527038</v>
+        <v>0.05526038266990106</v>
       </c>
       <c r="F47" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G47" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H47" t="n">
-        <v>0.8650726094794059</v>
+        <v>0.8665159381496877</v>
       </c>
       <c r="I47" t="n">
-        <v>0.06610255587800465</v>
+        <v>0.06621294107755255</v>
       </c>
       <c r="J47" t="n">
-        <v>19.94700379559461</v>
+        <v>19.94698980604132</v>
       </c>
       <c r="K47" t="n">
-        <v>0.01265990738012182</v>
+        <v>0.0126599261837991</v>
       </c>
       <c r="L47" t="n">
-        <v>13.17719167610037</v>
+        <v>13.14829884034963</v>
       </c>
       <c r="M47" t="n">
-        <v>0.00836326236556822</v>
+        <v>0.008344942990392625</v>
       </c>
     </row>
     <row r="48">
@@ -27309,40 +27309,40 @@
         <v>22.48889120165342</v>
       </c>
       <c r="B48" t="n">
-        <v>20.37842355013544</v>
+        <v>20.35105198561671</v>
       </c>
       <c r="C48" t="n">
-        <v>15.0000005805079</v>
+        <v>15.0000006162776</v>
       </c>
       <c r="D48" t="n">
-        <v>0.04728305346467807</v>
+        <v>0.04728312250446798</v>
       </c>
       <c r="E48" t="n">
-        <v>0.04937852576659869</v>
+        <v>0.04937859901486435</v>
       </c>
       <c r="F48" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G48" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H48" t="n">
-        <v>0.8380099875357875</v>
+        <v>0.839539989361015</v>
       </c>
       <c r="I48" t="n">
-        <v>0.0594061595097412</v>
+        <v>0.05951470742397452</v>
       </c>
       <c r="J48" t="n">
-        <v>19.94700326021815</v>
+        <v>19.94698926657876</v>
       </c>
       <c r="K48" t="n">
-        <v>0.01174484009971319</v>
+        <v>0.01174485754184093</v>
       </c>
       <c r="L48" t="n">
-        <v>11.91477267448691</v>
+        <v>11.87630680420201</v>
       </c>
       <c r="M48" t="n">
-        <v>0.007015444779385393</v>
+        <v>0.006992811279657983</v>
       </c>
     </row>
     <row r="49">
@@ -27350,40 +27350,40 @@
         <v>23.32269542113314</v>
       </c>
       <c r="B49" t="n">
-        <v>21.2151604872324</v>
+        <v>21.18410799426041</v>
       </c>
       <c r="C49" t="n">
-        <v>14.99990101205649</v>
+        <v>14.99993554635113</v>
       </c>
       <c r="D49" t="n">
-        <v>0.0423906953021292</v>
+        <v>0.04239085469361716</v>
       </c>
       <c r="E49" t="n">
-        <v>0.04426934994382078</v>
+        <v>0.04426951742909337</v>
       </c>
       <c r="F49" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G49" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H49" t="n">
-        <v>0.8132834690993092</v>
+        <v>0.8148940751754532</v>
       </c>
       <c r="I49" t="n">
-        <v>0.05360469540192144</v>
+        <v>0.0537109310862945</v>
       </c>
       <c r="J49" t="n">
-        <v>19.94687085407495</v>
+        <v>19.94690273664067</v>
       </c>
       <c r="K49" t="n">
-        <v>0.01092000484291376</v>
+        <v>0.01092004617522854</v>
       </c>
       <c r="L49" t="n">
-        <v>10.71932889184823</v>
+        <v>10.67152616782109</v>
       </c>
       <c r="M49" t="n">
-        <v>0.005868345178955971</v>
+        <v>0.005842188135740206</v>
       </c>
     </row>
     <row r="50">
@@ -27391,40 +27391,40 @@
         <v>24.16037719913241</v>
       </c>
       <c r="B50" t="n">
-        <v>22.03670716125609</v>
+        <v>22.00211079838838</v>
       </c>
       <c r="C50" t="n">
-        <v>15.00037197213928</v>
+        <v>15.00040260426613</v>
       </c>
       <c r="D50" t="n">
-        <v>0.03813372819586849</v>
+        <v>0.03813386165810639</v>
       </c>
       <c r="E50" t="n">
-        <v>0.03982372419545227</v>
+        <v>0.03982386449892376</v>
       </c>
       <c r="F50" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G50" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H50" t="n">
-        <v>0.7907169411203248</v>
+        <v>0.7923997353469615</v>
       </c>
       <c r="I50" t="n">
-        <v>0.04856596159882327</v>
+        <v>0.04866939003853319</v>
       </c>
       <c r="J50" t="n">
-        <v>19.94749713687116</v>
+        <v>19.9475238298963</v>
       </c>
       <c r="K50" t="n">
-        <v>0.01017622093433081</v>
+        <v>0.01017625680345496</v>
       </c>
       <c r="L50" t="n">
-        <v>9.586949583908629</v>
+        <v>9.529978742876153</v>
       </c>
       <c r="M50" t="n">
-        <v>0.004890784863020039</v>
+        <v>0.004861731804206535</v>
       </c>
     </row>
     <row r="51">
@@ -27432,40 +27432,40 @@
         <v>25</v>
       </c>
       <c r="B51" t="n">
-        <v>22.84273725724368</v>
+        <v>22.8047293491375</v>
       </c>
       <c r="C51" t="n">
-        <v>15.00015971651553</v>
+        <v>15.00017992449046</v>
       </c>
       <c r="D51" t="n">
-        <v>0.03441868125646921</v>
+        <v>0.03441877779878579</v>
       </c>
       <c r="E51" t="n">
-        <v>0.03594403522489352</v>
+        <v>0.03594413688197859</v>
       </c>
       <c r="F51" t="n">
-        <v>7.499246066984532</v>
+        <v>7.499251520370041</v>
       </c>
       <c r="G51" t="n">
-        <v>95.11698197166699</v>
+        <v>95.11705113989623</v>
       </c>
       <c r="H51" t="n">
-        <v>0.7700669133092013</v>
+        <v>0.7718163835860929</v>
       </c>
       <c r="I51" t="n">
-        <v>0.0441740090376508</v>
+        <v>0.04427442994323707</v>
       </c>
       <c r="J51" t="n">
-        <v>19.9472148793075</v>
+        <v>19.94722771050212</v>
       </c>
       <c r="K51" t="n">
-        <v>0.009504029711246257</v>
+        <v>0.009504056606603918</v>
       </c>
       <c r="L51" t="n">
-        <v>8.511893125600126</v>
+        <v>8.445959639190546</v>
       </c>
       <c r="M51" t="n">
-        <v>0.004055567940393334</v>
+        <v>0.004024162137864236</v>
       </c>
     </row>
   </sheetData>
@@ -27479,7 +27479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27804,7 +27804,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>24335.34305355373</v>
+        <v>24335.32616124057</v>
       </c>
       <c r="C7" t="n">
         <v>-7.088526180019682</v>
@@ -27816,13 +27816,13 @@
         <v>5.094493537559762</v>
       </c>
       <c r="F7" t="n">
-        <v>17849.70968062918</v>
+        <v>17849.69729030104</v>
       </c>
       <c r="G7" t="n">
-        <v>8924.854840314589</v>
+        <v>8924.848645150521</v>
       </c>
       <c r="H7" t="n">
-        <v>8924.854840314589</v>
+        <v>8924.848645150521</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -27834,19 +27834,19 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>649348.3887775004</v>
+        <v>649347.9380340567</v>
       </c>
       <c r="M7" t="n">
-        <v>1863303.981020963</v>
+        <v>1863302.687613498</v>
       </c>
       <c r="N7" t="n">
-        <v>1231805.301924092</v>
+        <v>1231804.446869743</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>877881.0882559151</v>
+        <v>877880.4788771106</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -28460,220 +28460,275 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>yaw</t>
+          <t>Above_yaw</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>28279.92605501719</v>
+        <v>645370.2694899647</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>-4.720121143165096</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>-0.1464296349733888</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>4.275123515940753</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>9435311.138557643</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>9798039.488938248</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>9771315.540437723</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>446057.7398755032</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1957666.832804562</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>-232316.4393010359</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>21244375.52600597</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>35971821.14191036</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>24163708.39734823</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>1.746229827404022e-10</v>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>14980658.61691782</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>171688.4316270081</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>nacelle</t>
+          <t>yaw</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>673650.212437295</v>
+        <v>28279.92605501719</v>
       </c>
       <c r="C20" t="n">
-        <v>-4.521969885394927</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.140282495632538</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>4.095653279260515</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>15273218.10699867</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>14410593.68847589</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>13760301.12176793</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>498291.8736498476</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>2566116.606573524</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>-254252.731971464</v>
+        <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>26586536.80016926</v>
+        <v>0</v>
       </c>
       <c r="M20" t="n">
-        <v>39485597.61704023</v>
+        <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>27548500.1228249</v>
+        <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>70959.6917661003</v>
+        <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>15042402.00607398</v>
+        <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>132791.9623593269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Blades</t>
+          <t>nacelle</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>209601.9928202963</v>
+        <v>673650.1955449819</v>
       </c>
       <c r="C21" t="n">
-        <v>-11.40758121099564</v>
+        <v>-4.521969821036491</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>-0.1402824991502329</v>
       </c>
       <c r="E21" t="n">
-        <v>5.548444513660863</v>
+        <v>4.095653254213802</v>
       </c>
       <c r="F21" t="n">
-        <v>355032430.9018697</v>
+        <v>9910245.76528684</v>
       </c>
       <c r="G21" t="n">
-        <v>177516215.4509349</v>
+        <v>10850691.4867255</v>
       </c>
       <c r="H21" t="n">
-        <v>177516215.4509349</v>
+        <v>10350145.96298178</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>428118.2775068661</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>2481422.952591601</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>-216068.2509369408</v>
       </c>
       <c r="L21" t="n">
-        <v>359545500.2180229</v>
+        <v>21223564.03722221</v>
       </c>
       <c r="M21" t="n">
-        <v>211244979.451032</v>
+        <v>35925694.25620393</v>
       </c>
       <c r="N21" t="n">
-        <v>206731910.1348787</v>
+        <v>24138344.22685292</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>786.101705076755</v>
       </c>
       <c r="P21" t="n">
-        <v>-5187230.258611443</v>
+        <v>14957707.78537402</v>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>170976.4410269023</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Blades</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>208647.4842374761</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-11.40759325172058</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>5.54844577919205</v>
+      </c>
+      <c r="F22" t="n">
+        <v>355464624.2400011</v>
+      </c>
+      <c r="G22" t="n">
+        <v>177732312.1200006</v>
+      </c>
+      <c r="H22" t="n">
+        <v>177732312.1200006</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>359945950.5984573</v>
+      </c>
+      <c r="M22" t="n">
+        <v>211307538.6169265</v>
+      </c>
+      <c r="N22" t="n">
+        <v>206826212.2584704</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>-5270092.801736692</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>Hub_System</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>68780.35223999179</v>
-      </c>
-      <c r="C22" t="n">
-        <v>-11.40758121099564</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>5.548444513660863</v>
-      </c>
-      <c r="F22" t="n">
-        <v>965925.6423689054</v>
-      </c>
-      <c r="G22" t="n">
-        <v>608250.9362102973</v>
-      </c>
-      <c r="H22" t="n">
-        <v>608250.9362102973</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>3079437.028843469</v>
-      </c>
-      <c r="M22" t="n">
-        <v>11676257.67284088</v>
-      </c>
-      <c r="N22" t="n">
-        <v>9562746.286366323</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" t="n">
-        <v>4316224.03094611</v>
-      </c>
-      <c r="Q22" t="n">
+      <c r="B23" t="n">
+        <v>68748.63987161352</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-11.40759325172058</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>5.54844577919205</v>
+      </c>
+      <c r="F23" t="n">
+        <v>965286.2689963281</v>
+      </c>
+      <c r="G23" t="n">
+        <v>608070.789968377</v>
+      </c>
+      <c r="H23" t="n">
+        <v>608070.789968377</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>3077827.365785852</v>
+      </c>
+      <c r="M23" t="n">
+        <v>11670994.28257967</v>
+      </c>
+      <c r="N23" t="n">
+        <v>9558453.185790146</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>4314270.14254929</v>
+      </c>
+      <c r="Q23" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
incorporating new tower design into repo and regenerating HydrDyn files
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>69549.16141249203</v>
+        <v>69.54916141249203</v>
       </c>
     </row>
     <row r="27">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>21788.17237526133</v>
+        <v>21.78817237526133</v>
       </c>
     </row>
     <row r="28">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>368839.4071518108</v>
+        <v>368.8394071518107</v>
       </c>
     </row>
     <row r="29">
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>673650.1955449819</v>
+        <v>673.6501955449819</v>
       </c>
     </row>
     <row r="30">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>951046.3196540715</v>
+        <v>951.0463196540715</v>
       </c>
     </row>
     <row r="31">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>853493.3526021612</v>
+        <v>853.4933526021613</v>
       </c>
     </row>
     <row r="32">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1309947.640917867</v>
+        <v>1309.947640917867</v>
       </c>
     </row>
   </sheetData>
@@ -27479,7 +27479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28730,6 +28730,61 @@
       </c>
       <c r="Q23" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>RNA</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>951046.3196540715</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-6.530331782251217</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0.09936564711008664</v>
+      </c>
+      <c r="E24" t="n">
+        <v>4.519396038592809</v>
+      </c>
+      <c r="F24" t="n">
+        <v>484796980.8754737</v>
+      </c>
+      <c r="G24" t="n">
+        <v>318905664.1432217</v>
+      </c>
+      <c r="H24" t="n">
+        <v>319940121.0152207</v>
+      </c>
+      <c r="I24" t="n">
+        <v>617911.1599562053</v>
+      </c>
+      <c r="J24" t="n">
+        <v>-14066492.87659087</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-256112.5089031481</v>
+      </c>
+      <c r="L24" t="n">
+        <v>384247342.0014653</v>
+      </c>
+      <c r="M24" t="n">
+        <v>258904227.1557102</v>
+      </c>
+      <c r="N24" t="n">
+        <v>240523009.6711134</v>
+      </c>
+      <c r="O24" t="n">
+        <v>786.101705076755</v>
+      </c>
+      <c r="P24" t="n">
+        <v>14001885.12618663</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>170976.4410269023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct floating tower z values to go up to tower top, not hub height
</commit_message>
<xml_diff>
--- a/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
+++ b/Documentation/IEA-15-240-RWT_FineGrid_tabular.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbarter/devel/IEA-15-240-RWT/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5433525D-9549-9D46-B76C-6425E29D071A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D75DE82-F732-F345-8A2D-93C056BC99E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview Fixed-Bottom" sheetId="1" r:id="rId1"/>
@@ -27725,7 +27725,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27878,7 +27878,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>28.564</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -27910,7 +27910,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>28.565000000000001</v>
+        <v>28.001000000000001</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -27942,7 +27942,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>28.574000000000002</v>
+        <v>28.01</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -27974,7 +27974,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>28.574999999999999</v>
+        <v>28.010999999999999</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -28006,7 +28006,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>42.128</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -28038,7 +28038,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>42.128999999999998</v>
+        <v>41.000999999999998</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -28070,7 +28070,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>42.139000000000003</v>
+        <v>41.01</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -28102,7 +28102,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12">
-        <v>42.14</v>
+        <v>41.011000000000003</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -28134,7 +28134,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13">
-        <v>55.692</v>
+        <v>54</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -28166,7 +28166,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14">
-        <v>55.692999999999998</v>
+        <v>54.000999999999998</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -28198,7 +28198,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15">
-        <v>55.703000000000003</v>
+        <v>54.01</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -28230,7 +28230,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16">
-        <v>55.704000000000001</v>
+        <v>54.011000000000003</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -28262,7 +28262,7 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17">
-        <v>69.256</v>
+        <v>67</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -28294,7 +28294,7 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18">
-        <v>69.257000000000005</v>
+        <v>67.001000000000005</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -28326,7 +28326,7 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19">
-        <v>69.266999999999996</v>
+        <v>67.010000000000005</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -28358,7 +28358,7 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20">
-        <v>69.268000000000001</v>
+        <v>67.010999999999996</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -28390,7 +28390,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21">
-        <v>82.82</v>
+        <v>80</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -28422,7 +28422,7 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22">
-        <v>82.820999999999998</v>
+        <v>80.001000000000005</v>
       </c>
       <c r="C22">
         <v>10</v>
@@ -28454,7 +28454,7 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23">
-        <v>82.831000000000003</v>
+        <v>80.010000000000005</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -28486,7 +28486,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24">
-        <v>82.831999999999994</v>
+        <v>80.010999999999996</v>
       </c>
       <c r="C24">
         <v>10</v>
@@ -28518,7 +28518,7 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25">
-        <v>96.384</v>
+        <v>93</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -28550,7 +28550,7 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26">
-        <v>96.385000000000005</v>
+        <v>93.001000000000005</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -28582,7 +28582,7 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27">
-        <v>96.394999999999996</v>
+        <v>93.01</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -28614,7 +28614,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28">
-        <v>96.396000000000001</v>
+        <v>93.010999999999996</v>
       </c>
       <c r="C28">
         <v>10</v>
@@ -28646,7 +28646,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29">
-        <v>109.94799999999999</v>
+        <v>106</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -28678,7 +28678,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30">
-        <v>109.949</v>
+        <v>106.001</v>
       </c>
       <c r="C30">
         <v>10</v>
@@ -28710,7 +28710,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31">
-        <v>109.959</v>
+        <v>106.01</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -28742,7 +28742,7 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32">
-        <v>109.96</v>
+        <v>106.011</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -28774,7 +28774,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B33">
-        <v>123.51300000000001</v>
+        <v>119</v>
       </c>
       <c r="C33">
         <v>9.7850000000000001</v>
@@ -28806,7 +28806,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B34">
-        <v>123.514</v>
+        <v>119.001</v>
       </c>
       <c r="C34">
         <v>9.7850000000000001</v>
@@ -28838,7 +28838,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B35">
-        <v>123.523</v>
+        <v>119.01</v>
       </c>
       <c r="C35">
         <v>9.7850000000000001</v>
@@ -28870,7 +28870,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B36">
-        <v>123.524</v>
+        <v>119.011</v>
       </c>
       <c r="C36">
         <v>9.7850000000000001</v>
@@ -28902,7 +28902,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B37">
-        <v>137.077</v>
+        <v>132</v>
       </c>
       <c r="C37">
         <v>7.0609999999999999</v>
@@ -28934,7 +28934,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B38">
-        <v>137.078</v>
+        <v>132.001</v>
       </c>
       <c r="C38">
         <v>7.0609999999999999</v>
@@ -28966,7 +28966,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B39">
-        <v>137.08699999999999</v>
+        <v>132.01</v>
       </c>
       <c r="C39">
         <v>7.0579999999999998</v>
@@ -28998,7 +28998,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B40">
-        <v>137.08799999999999</v>
+        <v>132.011</v>
       </c>
       <c r="C40">
         <v>7.0579999999999998</v>
@@ -29033,7 +29033,7 @@
         <v>195</v>
       </c>
       <c r="B41">
-        <v>150</v>
+        <v>144.386</v>
       </c>
       <c r="C41">
         <v>6.5</v>

</xml_diff>